<commit_message>
New implementaion of patterns
DID SHIT ITZ ALL GD NOW!!!
</commit_message>
<xml_diff>
--- a/ProjectIR/Assets/Resources/Models/Obstacle Resources/obstaclePatterns.xlsx
+++ b/ProjectIR/Assets/Resources/Models/Obstacle Resources/obstaclePatterns.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Pattern 1:</t>
   </si>
@@ -31,6 +31,18 @@
   </si>
   <si>
     <t>total blocks</t>
+  </si>
+  <si>
+    <t>Pattern 3:</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>advanced</t>
+  </si>
+  <si>
+    <t>painful</t>
   </si>
 </sst>
 </file>
@@ -462,23 +474,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AG37"/>
+  <dimension ref="A2:AX37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
       <c r="S2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>-3</v>
       </c>
@@ -566,8 +590,51 @@
       <c r="AG4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>-2.5</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AT4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AU4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AV4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -602,8 +669,26 @@
       </c>
       <c r="AD5" s="4"/>
       <c r="AE5" s="7"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="7"/>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.1</v>
       </c>
@@ -638,8 +723,26 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="8"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI6">
+        <v>0.1</v>
+      </c>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="8"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.2</v>
       </c>
@@ -672,8 +775,26 @@
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="8"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI7">
+        <v>0.2</v>
+      </c>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="8"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.3</v>
       </c>
@@ -710,8 +831,26 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="8"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI8">
+        <v>0.3</v>
+      </c>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="8"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.4</v>
       </c>
@@ -744,8 +883,26 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="8"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI9">
+        <v>0.4</v>
+      </c>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="8"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -784,8 +941,24 @@
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="8"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="8"/>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.6</v>
       </c>
@@ -818,8 +991,24 @@
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="8"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI11">
+        <v>0.6</v>
+      </c>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="8"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.7</v>
       </c>
@@ -858,8 +1047,24 @@
         <v>1</v>
       </c>
       <c r="AE12" s="8"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI12">
+        <v>0.7</v>
+      </c>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="8"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.8</v>
       </c>
@@ -892,8 +1097,26 @@
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
       <c r="AE13" s="8"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI13">
+        <v>0.8</v>
+      </c>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="8"/>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.9</v>
       </c>
@@ -930,8 +1153,26 @@
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AE14" s="8"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI14">
+        <v>0.9</v>
+      </c>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="8"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -964,8 +1205,26 @@
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
       <c r="AE15" s="8"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="8"/>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.1000000000000001</v>
       </c>
@@ -1004,8 +1263,26 @@
       </c>
       <c r="AD16" s="2"/>
       <c r="AE16" s="8"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV16" s="8"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.2</v>
       </c>
@@ -1038,8 +1315,26 @@
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="8"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI17">
+        <v>1.2</v>
+      </c>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.3</v>
       </c>
@@ -1076,8 +1371,24 @@
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
       <c r="AE18" s="8"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI18">
+        <v>1.3</v>
+      </c>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
+      <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="8"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.4</v>
       </c>
@@ -1110,8 +1421,24 @@
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
       <c r="AE19" s="8"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI19">
+        <v>1.4</v>
+      </c>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2"/>
+      <c r="AO19" s="2"/>
+      <c r="AP19" s="2"/>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="8"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.5</v>
       </c>
@@ -1146,8 +1473,26 @@
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
       <c r="AE20" s="8"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI20">
+        <v>1.5</v>
+      </c>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
+      <c r="AN20" s="2"/>
+      <c r="AO20" s="2"/>
+      <c r="AP20" s="2"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS20" s="2"/>
+      <c r="AT20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="8"/>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.6</v>
       </c>
@@ -1182,8 +1527,24 @@
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="8"/>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI21">
+        <v>1.6</v>
+      </c>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="8"/>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.7</v>
       </c>
@@ -1218,8 +1579,26 @@
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
       <c r="AE22" s="8"/>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI22">
+        <v>1.7</v>
+      </c>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="8"/>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.8</v>
       </c>
@@ -1254,8 +1633,26 @@
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
       <c r="AE23" s="8"/>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI23">
+        <v>1.8</v>
+      </c>
+      <c r="AJ23" s="5"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.9</v>
       </c>
@@ -1290,8 +1687,26 @@
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
       <c r="AE24" s="8"/>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI24">
+        <v>1.9</v>
+      </c>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="8"/>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1326,8 +1741,26 @@
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
       <c r="AE25" s="8"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI25">
+        <v>2</v>
+      </c>
+      <c r="AJ25" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="8"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2.1</v>
       </c>
@@ -1362,8 +1795,26 @@
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
       <c r="AE26" s="8"/>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI26">
+        <v>2.1</v>
+      </c>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="8"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2.2000000000000002</v>
       </c>
@@ -1398,8 +1849,24 @@
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AE27" s="8"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+      <c r="AP27" s="2"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="8"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2.2999999999999998</v>
       </c>
@@ -1434,8 +1901,26 @@
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
       <c r="AE28" s="8"/>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="2"/>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
+      <c r="AP28" s="2"/>
+      <c r="AQ28" s="2"/>
+      <c r="AR28" s="2"/>
+      <c r="AS28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="8"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2.4</v>
       </c>
@@ -1470,8 +1955,24 @@
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="8"/>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI29">
+        <v>2.4</v>
+      </c>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="8"/>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2.5</v>
       </c>
@@ -1506,8 +2007,26 @@
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>
       <c r="AE30" s="8"/>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI30">
+        <v>2.5</v>
+      </c>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+      <c r="AO30" s="2"/>
+      <c r="AP30" s="2"/>
+      <c r="AQ30" s="2"/>
+      <c r="AR30" s="2"/>
+      <c r="AS30" s="2"/>
+      <c r="AT30" s="2"/>
+      <c r="AU30" s="2"/>
+      <c r="AV30" s="8"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2.6</v>
       </c>
@@ -1542,8 +2061,24 @@
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
       <c r="AE31" s="8"/>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI31">
+        <v>2.6</v>
+      </c>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="2"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="2"/>
+      <c r="AN31" s="2"/>
+      <c r="AO31" s="2"/>
+      <c r="AP31" s="2"/>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="2"/>
+      <c r="AS31" s="2"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
+      <c r="AV31" s="8"/>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2.7</v>
       </c>
@@ -1578,8 +2113,26 @@
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
       <c r="AE32" s="8"/>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI32">
+        <v>2.7</v>
+      </c>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="8"/>
+    </row>
+    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2.8</v>
       </c>
@@ -1614,8 +2167,24 @@
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
       <c r="AE33" s="8"/>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI33">
+        <v>2.8</v>
+      </c>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="2"/>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="2"/>
+      <c r="AS33" s="2"/>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="2"/>
+      <c r="AV33" s="8"/>
+    </row>
+    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2.9</v>
       </c>
@@ -1650,8 +2219,26 @@
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
       <c r="AE34" s="8"/>
-    </row>
-    <row r="35" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI34">
+        <v>2.9</v>
+      </c>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="2"/>
+      <c r="AT34" s="2"/>
+      <c r="AU34" s="2"/>
+      <c r="AV34" s="8"/>
+    </row>
+    <row r="35" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1686,8 +2273,24 @@
       <c r="AC35" s="12"/>
       <c r="AD35" s="12"/>
       <c r="AE35" s="13"/>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI35">
+        <v>3</v>
+      </c>
+      <c r="AJ35" s="11"/>
+      <c r="AK35" s="12"/>
+      <c r="AL35" s="12"/>
+      <c r="AM35" s="12"/>
+      <c r="AN35" s="12"/>
+      <c r="AO35" s="12"/>
+      <c r="AP35" s="12"/>
+      <c r="AQ35" s="12"/>
+      <c r="AR35" s="12"/>
+      <c r="AS35" s="12"/>
+      <c r="AT35" s="12"/>
+      <c r="AU35" s="12"/>
+      <c r="AV35" s="13"/>
+    </row>
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -1707,6 +2310,16 @@
       <c r="AD37">
         <f>SUM(S5:AE34)</f>
         <v>17</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU37">
+        <f>SUM(AJ5:AV34)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>